<commit_message>
update file label lagi
</commit_message>
<xml_diff>
--- a/04 - PERKULIAHAN/Label Untuk Map Absen.xlsx
+++ b/04 - PERKULIAHAN/Label Untuk Map Absen.xlsx
@@ -649,7 +649,7 @@
   <dimension ref="A3:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3913,36 +3913,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E86:G86"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="85" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>